<commit_message>
added initial file validation
</commit_message>
<xml_diff>
--- a/01-getting-started/src/python/data_tables/shopdata.xlsx
+++ b/01-getting-started/src/python/data_tables/shopdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\cohort4\01-getting-started\src\python\data_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F257C6-7198-4AC4-884F-41A47CE39CB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A4CC51-916C-474B-8875-9544876DEE5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{F1C56F83-F90B-4560-ABD0-990105EB406D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{F1C56F83-F90B-4560-ABD0-990105EB406D}"/>
   </bookViews>
   <sheets>
     <sheet name="customer" sheetId="3" r:id="rId1"/>
@@ -644,9 +644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BF163BA-DBA3-44B9-9B8A-227C2AFC644E}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1988,7 +1986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{132F85FD-BF9B-4362-B4A3-D63B0FA39E61}">
   <dimension ref="A1:C301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A32" sqref="A32:A301"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
exception code for loading merged data
</commit_message>
<xml_diff>
--- a/01-getting-started/src/python/data_tables/shopdata.xlsx
+++ b/01-getting-started/src/python/data_tables/shopdata.xlsx
@@ -675,7 +675,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="105">
+  <dataValidations count="125">
     <dataValidation sqref="D2:D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
       <formula1>ISNUMBER(MATCH("*@*.?*",D2,0))</formula1>
     </dataValidation>
@@ -688,6 +688,61 @@
       <formula2>9999999999</formula2>
     </dataValidation>
     <dataValidation sqref="E2:E11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole">
+      <formula1>1000000000</formula1>
+      <formula2>9999999999</formula2>
+    </dataValidation>
+    <dataValidation sqref="A2:A11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="B2:C11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>ISNUMBER(MATCH("*@*.?*",D2,0))</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole" operator="between">
+      <formula1>1000000000</formula1>
+      <formula2>9999999999</formula2>
+    </dataValidation>
+    <dataValidation sqref="A2:A11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="B2:C11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>ISNUMBER(MATCH("*@*.?*",D2,0))</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole" operator="between">
+      <formula1>1000000000</formula1>
+      <formula2>9999999999</formula2>
+    </dataValidation>
+    <dataValidation sqref="A2:A11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="B2:C11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>ISNUMBER(MATCH("*@*.?*",D2,0))</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole" operator="between">
+      <formula1>1000000000</formula1>
+      <formula2>9999999999</formula2>
+    </dataValidation>
+    <dataValidation sqref="A2:A11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="B2:C11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>ISNUMBER(MATCH("*@*.?*",D2,0))</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole" operator="between">
+      <formula1>1000000000</formula1>
+      <formula2>9999999999</formula2>
+    </dataValidation>
+    <dataValidation sqref="A2:A11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="B2:C11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>ISNUMBER(MATCH("*@*.?*",D2,0))</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole" operator="between">
       <formula1>1000000000</formula1>
       <formula2>9999999999</formula2>
     </dataValidation>
@@ -2111,10 +2166,30 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="50">
+  <dataValidations count="60">
     <dataValidation sqref="A2:B101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
     <dataValidation sqref="C2:C101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="date" operator="lessThan">
       <formula1>DATEVALUE("1/1/2021")</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:B101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="C2:C101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="date" operator="lessThan">
+      <formula1>DATEVALUE("2021/1/1")</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:B101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="C2:C101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="date" operator="lessThan">
+      <formula1>DATEVALUE("2021/1/1")</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:B101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="C2:C101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="date" operator="lessThan">
+      <formula1>DATEVALUE("2021/1/1")</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:B101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="C2:C101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="date" operator="lessThan">
+      <formula1>DATEVALUE("2021/1/1")</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:B101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="C2:C101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="date" operator="lessThan">
+      <formula1>DATEVALUE("2021/1/1")</formula1>
     </dataValidation>
     <dataValidation sqref="A2:B101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
     <dataValidation sqref="C2:C101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="date" operator="lessThan">
@@ -5555,7 +5630,12 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="24">
+  <dataValidations count="29">
+    <dataValidation sqref="A2:C301" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="A2:C301" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="A2:C301" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="A2:C301" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="A2:C301" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
     <dataValidation sqref="A2:C301" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
     <dataValidation sqref="A2:C301" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
     <dataValidation sqref="A2:C301" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
@@ -5778,7 +5858,27 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="52">
+  <dataValidations count="62">
+    <dataValidation sqref="B2:B13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A13 C2:C13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="B2:B13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A13 C2:C13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="B2:B13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A13 C2:C13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="B2:B13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A13 C2:C13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="B2:B13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A13 C2:C13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
     <dataValidation sqref="B2:B13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
       <formula1>100</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
finished most of the testing
</commit_message>
<xml_diff>
--- a/01-getting-started/src/python/data_tables/shopdata.xlsx
+++ b/01-getting-started/src/python/data_tables/shopdata.xlsx
@@ -675,7 +675,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="125">
+  <dataValidations count="149">
     <dataValidation sqref="D2:D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
       <formula1>ISNUMBER(MATCH("*@*.?*",D2,0))</formula1>
     </dataValidation>
@@ -688,6 +688,72 @@
       <formula2>9999999999</formula2>
     </dataValidation>
     <dataValidation sqref="E2:E11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole">
+      <formula1>1000000000</formula1>
+      <formula2>9999999999</formula2>
+    </dataValidation>
+    <dataValidation sqref="A2:A11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="B2:C11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>ISNUMBER(MATCH("*@*.?*",D2,0))</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole" operator="between">
+      <formula1>1000000000</formula1>
+      <formula2>9999999999</formula2>
+    </dataValidation>
+    <dataValidation sqref="A2:A11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="B2:C11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>ISNUMBER(MATCH("*@*.?*",D2,0))</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole" operator="between">
+      <formula1>1000000000</formula1>
+      <formula2>9999999999</formula2>
+    </dataValidation>
+    <dataValidation sqref="A2:A11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="B2:C11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>ISNUMBER(MATCH("*@*.?*",D2,0))</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole" operator="between">
+      <formula1>1000000000</formula1>
+      <formula2>9999999999</formula2>
+    </dataValidation>
+    <dataValidation sqref="A2:A11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="B2:C11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>ISNUMBER(MATCH("*@*.?*",D2,0))</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole" operator="between">
+      <formula1>1000000000</formula1>
+      <formula2>9999999999</formula2>
+    </dataValidation>
+    <dataValidation sqref="A2:A11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="B2:C11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>ISNUMBER(MATCH("*@*.?*",D2,0))</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole" operator="between">
+      <formula1>1000000000</formula1>
+      <formula2>9999999999</formula2>
+    </dataValidation>
+    <dataValidation sqref="A2:A11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="B2:C11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="custom">
+      <formula1>ISNUMBER(MATCH("*@*.?*",D2,0))</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E11" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole" operator="between">
       <formula1>1000000000</formula1>
       <formula2>9999999999</formula2>
     </dataValidation>
@@ -2166,10 +2232,34 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="60">
+  <dataValidations count="72">
     <dataValidation sqref="A2:B101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
     <dataValidation sqref="C2:C101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="date" operator="lessThan">
       <formula1>DATEVALUE("1/1/2021")</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:B101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="C2:C101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="date" operator="lessThan">
+      <formula1>DATEVALUE("2021/1/1")</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:B101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="C2:C101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="date" operator="lessThan">
+      <formula1>DATEVALUE("2021/1/1")</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:B101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="C2:C101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="date" operator="lessThan">
+      <formula1>DATEVALUE("2021/1/1")</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:B101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="C2:C101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="date" operator="lessThan">
+      <formula1>DATEVALUE("2021/1/1")</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:B101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="C2:C101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="date" operator="lessThan">
+      <formula1>DATEVALUE("2021/1/1")</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:B101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="C2:C101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="date" operator="lessThan">
+      <formula1>DATEVALUE("2021/1/1")</formula1>
     </dataValidation>
     <dataValidation sqref="A2:B101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
     <dataValidation sqref="C2:C101" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="date" operator="lessThan">
@@ -5630,7 +5720,13 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="29">
+  <dataValidations count="35">
+    <dataValidation sqref="A2:C301" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="A2:C301" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="A2:C301" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="A2:C301" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="A2:C301" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="A2:C301" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
     <dataValidation sqref="A2:C301" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
     <dataValidation sqref="A2:C301" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
     <dataValidation sqref="A2:C301" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
@@ -5858,7 +5954,31 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="62">
+  <dataValidations count="74">
+    <dataValidation sqref="B2:B13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A13 C2:C13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="B2:B13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A13 C2:C13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="B2:B13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A13 C2:C13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="B2:B13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A13 C2:C13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="B2:B13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A13 C2:C13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
+    <dataValidation sqref="B2:B13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
+      <formula1>100</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A13 C2:C13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="whole"/>
     <dataValidation sqref="B2:B13" showErrorMessage="1" showInputMessage="1" allowBlank="0" type="textLength" operator="lessThanOrEqual">
       <formula1>100</formula1>
     </dataValidation>

</xml_diff>